<commit_message>
2022-09-07 15:27 Interview Page + Beginning of report
</commit_message>
<xml_diff>
--- a/Interview Questions.xlsx
+++ b/Interview Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\scepanovicka\code\skoooty\job-prepr-ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11C9255-2909-47B4-B41A-7A2AA004CDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD4FDAB-854F-4A7E-84C7-0CB6E42D14F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E967EEF-5A21-4562-83B0-DA44B13E1A81}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8832" xr2:uid="{8E967EEF-5A21-4562-83B0-DA44B13E1A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="215">
   <si>
     <t>Area</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t>Why String is final in Java?</t>
+  </si>
+  <si>
+    <t>Piccolo</t>
+  </si>
+  <si>
+    <t>How many times did you orgasam last week?</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F485B2A5-2B3A-439F-A5FA-204D243FC066}">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B212"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2738,6 +2744,14 @@
         <v>212</v>
       </c>
     </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>